<commit_message>
fix 'invalid' def files
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_ChallengeQuestion_InvalidCaseField.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_ChallengeQuestion_InvalidCaseField.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleynoronha/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318A213C-92B7-2E41-A7DD-71699CD733F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38F720A-5366-6F42-948C-6FC1A510A4C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="16" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">CaseEvent!$A$22:$T$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseField!$A$3:$IO$123</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -55,7 +55,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -66,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6675" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6671" uniqueCount="1062">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3754,11 +3757,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -13324,7 +13329,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F59" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F58" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
@@ -15177,7 +15182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE0C02E-59B7-9148-BB65-087866DFAC16}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -15213,7 +15218,7 @@
       <c r="H1" s="531"/>
       <c r="I1" s="531"/>
     </row>
-    <row r="2" spans="1:9" ht="168" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="56" x14ac:dyDescent="0.15">
       <c r="A2" s="532" t="s">
         <v>5</v>
       </c>
@@ -15269,7 +15274,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="210" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="56" x14ac:dyDescent="0.15">
       <c r="A4" s="540"/>
       <c r="B4" s="17" t="s">
         <v>922</v>
@@ -15296,7 +15301,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="112" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="540"/>
       <c r="B5" s="17" t="s">
         <v>922</v>
@@ -15323,7 +15328,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="56" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="540"/>
       <c r="B6" s="17" t="s">
         <v>922</v>
@@ -15350,7 +15355,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="56" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="540"/>
       <c r="B7" s="17" t="s">
         <v>922</v>
@@ -36872,10 +36877,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:EK59"/>
+  <dimension ref="A1:EK58"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD51"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -36888,7 +36893,7 @@
     <col min="7" max="16384" width="8.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:141" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="198" t="s">
         <v>702</v>
       </c>
@@ -36904,7 +36909,7 @@
       <c r="E1" s="81"/>
       <c r="F1" s="81"/>
     </row>
-    <row r="2" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:141" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="163" t="s">
         <v>4</v>
       </c>
@@ -36924,7 +36929,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
         <v>9</v>
       </c>
@@ -36944,7 +36949,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="60">
         <v>42736</v>
       </c>
@@ -36962,7 +36967,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="60">
         <v>42736</v>
       </c>
@@ -36980,7 +36985,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="60">
         <v>42736</v>
       </c>
@@ -36998,7 +37003,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="60">
         <v>42736</v>
       </c>
@@ -37016,25 +37021,25 @@
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="60">
         <v>42736</v>
       </c>
       <c r="B8" s="81"/>
       <c r="C8" s="62" t="s">
-        <v>882</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>941</v>
+        <v>880</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>392</v>
       </c>
       <c r="E8" s="134" t="s">
-        <v>936</v>
+        <v>776</v>
       </c>
       <c r="F8" s="115" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="60">
         <v>42736</v>
       </c>
@@ -37042,8 +37047,8 @@
       <c r="C9" s="62" t="s">
         <v>880</v>
       </c>
-      <c r="D9" s="62" t="s">
-        <v>392</v>
+      <c r="D9" s="65" t="s">
+        <v>535</v>
       </c>
       <c r="E9" s="134" t="s">
         <v>776</v>
@@ -37052,16 +37057,16 @@
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="60">
         <v>42736</v>
       </c>
       <c r="B10" s="81"/>
-      <c r="C10" s="62" t="s">
-        <v>880</v>
-      </c>
-      <c r="D10" s="65" t="s">
-        <v>535</v>
+      <c r="C10" s="65" t="s">
+        <v>881</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>392</v>
       </c>
       <c r="E10" s="134" t="s">
         <v>776</v>
@@ -37070,43 +37075,43 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="65" t="s">
+    <row r="11" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="84"/>
+      <c r="C11" s="118" t="s">
         <v>881</v>
       </c>
-      <c r="D11" s="62" t="s">
-        <v>392</v>
+      <c r="D11" s="118" t="s">
+        <v>388</v>
       </c>
       <c r="E11" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F11" s="115" t="s">
+      <c r="F11" s="119" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="118" t="s">
+    <row r="12" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="81"/>
+      <c r="C12" s="120" t="s">
         <v>881</v>
       </c>
-      <c r="D12" s="118" t="s">
-        <v>388</v>
+      <c r="D12" s="120" t="s">
+        <v>373</v>
       </c>
       <c r="E12" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F12" s="119" t="s">
+      <c r="F12" s="115" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="60">
         <v>42736</v>
       </c>
@@ -37115,7 +37120,7 @@
         <v>881</v>
       </c>
       <c r="D13" s="120" t="s">
-        <v>373</v>
+        <v>542</v>
       </c>
       <c r="E13" s="134" t="s">
         <v>776</v>
@@ -37124,7 +37129,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="60">
         <v>42736</v>
       </c>
@@ -37133,7 +37138,7 @@
         <v>881</v>
       </c>
       <c r="D14" s="120" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E14" s="134" t="s">
         <v>776</v>
@@ -37142,57 +37147,192 @@
         <v>339</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="81"/>
+    <row r="15" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="84"/>
       <c r="C15" s="120" t="s">
         <v>881</v>
       </c>
       <c r="D15" s="120" t="s">
-        <v>544</v>
+        <v>953</v>
       </c>
       <c r="E15" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F15" s="115" t="s">
+      <c r="F15" s="119" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="84"/>
-      <c r="C16" s="120" t="s">
-        <v>881</v>
-      </c>
-      <c r="D16" s="120" t="s">
-        <v>953</v>
-      </c>
-      <c r="E16" s="134" t="s">
+    <row r="16" spans="1:141" s="288" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="339">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="332"/>
+      <c r="C16" s="289" t="s">
+        <v>922</v>
+      </c>
+      <c r="D16" s="289" t="s">
+        <v>924</v>
+      </c>
+      <c r="E16" s="355" t="s">
         <v>776</v>
       </c>
-      <c r="F16" s="119" t="s">
+      <c r="F16" s="354" t="s">
         <v>339</v>
       </c>
+      <c r="G16" s="389"/>
+      <c r="H16" s="389"/>
+      <c r="I16" s="389"/>
+      <c r="J16" s="389"/>
+      <c r="K16" s="389"/>
+      <c r="L16" s="389"/>
+      <c r="M16" s="389"/>
+      <c r="N16" s="389"/>
+      <c r="O16" s="389"/>
+      <c r="P16" s="389"/>
+      <c r="Q16" s="389"/>
+      <c r="R16" s="389"/>
+      <c r="S16" s="389"/>
+      <c r="T16" s="389"/>
+      <c r="U16" s="389"/>
+      <c r="V16" s="389"/>
+      <c r="W16" s="389"/>
+      <c r="X16" s="389"/>
+      <c r="Y16" s="389"/>
+      <c r="Z16" s="389"/>
+      <c r="AA16" s="389"/>
+      <c r="AB16" s="389"/>
+      <c r="AC16" s="389"/>
+      <c r="AD16" s="389"/>
+      <c r="AE16" s="389"/>
+      <c r="AF16" s="389"/>
+      <c r="AG16" s="389"/>
+      <c r="AH16" s="389"/>
+      <c r="AI16" s="389"/>
+      <c r="AJ16" s="389"/>
+      <c r="AK16" s="389"/>
+      <c r="AL16" s="389"/>
+      <c r="AM16" s="389"/>
+      <c r="AN16" s="389"/>
+      <c r="AO16" s="389"/>
+      <c r="AP16" s="389"/>
+      <c r="AQ16" s="389"/>
+      <c r="AR16" s="389"/>
+      <c r="AS16" s="389"/>
+      <c r="AT16" s="389"/>
+      <c r="AU16" s="389"/>
+      <c r="AV16" s="389"/>
+      <c r="AW16" s="389"/>
+      <c r="AX16" s="389"/>
+      <c r="AY16" s="389"/>
+      <c r="AZ16" s="389"/>
+      <c r="BA16" s="389"/>
+      <c r="BB16" s="389"/>
+      <c r="BC16" s="389"/>
+      <c r="BD16" s="389"/>
+      <c r="BE16" s="389"/>
+      <c r="BF16" s="389"/>
+      <c r="BG16" s="389"/>
+      <c r="BH16" s="389"/>
+      <c r="BI16" s="389"/>
+      <c r="BJ16" s="389"/>
+      <c r="BK16" s="389"/>
+      <c r="BL16" s="389"/>
+      <c r="BM16" s="389"/>
+      <c r="BN16" s="389"/>
+      <c r="BO16" s="389"/>
+      <c r="BP16" s="389"/>
+      <c r="BQ16" s="389"/>
+      <c r="BR16" s="389"/>
+      <c r="BS16" s="389"/>
+      <c r="BT16" s="389"/>
+      <c r="BU16" s="389"/>
+      <c r="BV16" s="389"/>
+      <c r="BW16" s="389"/>
+      <c r="BX16" s="389"/>
+      <c r="BY16" s="389"/>
+      <c r="BZ16" s="389"/>
+      <c r="CA16" s="389"/>
+      <c r="CB16" s="389"/>
+      <c r="CC16" s="389"/>
+      <c r="CD16" s="389"/>
+      <c r="CE16" s="389"/>
+      <c r="CF16" s="389"/>
+      <c r="CG16" s="389"/>
+      <c r="CH16" s="389"/>
+      <c r="CI16" s="389"/>
+      <c r="CJ16" s="389"/>
+      <c r="CK16" s="389"/>
+      <c r="CL16" s="389"/>
+      <c r="CM16" s="389"/>
+      <c r="CN16" s="389"/>
+      <c r="CO16" s="389"/>
+      <c r="CP16" s="389"/>
+      <c r="CQ16" s="389"/>
+      <c r="CR16" s="389"/>
+      <c r="CS16" s="389"/>
+      <c r="CT16" s="389"/>
+      <c r="CU16" s="389"/>
+      <c r="CV16" s="389"/>
+      <c r="CW16" s="389"/>
+      <c r="CX16" s="389"/>
+      <c r="CY16" s="389"/>
+      <c r="CZ16" s="389"/>
+      <c r="DA16" s="389"/>
+      <c r="DB16" s="389"/>
+      <c r="DC16" s="389"/>
+      <c r="DD16" s="389"/>
+      <c r="DE16" s="389"/>
+      <c r="DF16" s="389"/>
+      <c r="DG16" s="389"/>
+      <c r="DH16" s="389"/>
+      <c r="DI16" s="389"/>
+      <c r="DJ16" s="389"/>
+      <c r="DK16" s="389"/>
+      <c r="DL16" s="389"/>
+      <c r="DM16" s="389"/>
+      <c r="DN16" s="389"/>
+      <c r="DO16" s="389"/>
+      <c r="DP16" s="389"/>
+      <c r="DQ16" s="389"/>
+      <c r="DR16" s="389"/>
+      <c r="DS16" s="389"/>
+      <c r="DT16" s="389"/>
+      <c r="DU16" s="389"/>
+      <c r="DV16" s="389"/>
+      <c r="DW16" s="389"/>
+      <c r="DX16" s="389"/>
+      <c r="DY16" s="389"/>
+      <c r="DZ16" s="389"/>
+      <c r="EA16" s="389"/>
+      <c r="EB16" s="389"/>
+      <c r="EC16" s="389"/>
+      <c r="ED16" s="389"/>
+      <c r="EE16" s="389"/>
+      <c r="EF16" s="389"/>
+      <c r="EG16" s="389"/>
+      <c r="EH16" s="389"/>
+      <c r="EI16" s="389"/>
+      <c r="EJ16" s="389"/>
+      <c r="EK16" s="389"/>
     </row>
     <row r="17" spans="1:141" s="288" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="339">
-        <v>42736</v>
-      </c>
-      <c r="B17" s="332"/>
+      <c r="A17" s="286">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="287"/>
       <c r="C17" s="289" t="s">
         <v>922</v>
       </c>
       <c r="D17" s="289" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E17" s="355" t="s">
         <v>776</v>
       </c>
-      <c r="F17" s="354" t="s">
+      <c r="F17" s="290" t="s">
         <v>339</v>
       </c>
       <c r="G17" s="389"/>
@@ -37331,158 +37471,23 @@
       <c r="EJ17" s="389"/>
       <c r="EK17" s="389"/>
     </row>
-    <row r="18" spans="1:141" s="288" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="286">
-        <v>42736</v>
-      </c>
-      <c r="B18" s="287"/>
-      <c r="C18" s="289" t="s">
-        <v>922</v>
-      </c>
-      <c r="D18" s="289" t="s">
-        <v>923</v>
-      </c>
-      <c r="E18" s="355" t="s">
+    <row r="18" spans="1:141" s="432" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="462">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="465"/>
+      <c r="C18" s="464" t="s">
+        <v>983</v>
+      </c>
+      <c r="D18" s="385" t="s">
+        <v>996</v>
+      </c>
+      <c r="E18" s="493" t="s">
         <v>776</v>
       </c>
-      <c r="F18" s="290" t="s">
+      <c r="F18" s="494" t="s">
         <v>339</v>
       </c>
-      <c r="G18" s="389"/>
-      <c r="H18" s="389"/>
-      <c r="I18" s="389"/>
-      <c r="J18" s="389"/>
-      <c r="K18" s="389"/>
-      <c r="L18" s="389"/>
-      <c r="M18" s="389"/>
-      <c r="N18" s="389"/>
-      <c r="O18" s="389"/>
-      <c r="P18" s="389"/>
-      <c r="Q18" s="389"/>
-      <c r="R18" s="389"/>
-      <c r="S18" s="389"/>
-      <c r="T18" s="389"/>
-      <c r="U18" s="389"/>
-      <c r="V18" s="389"/>
-      <c r="W18" s="389"/>
-      <c r="X18" s="389"/>
-      <c r="Y18" s="389"/>
-      <c r="Z18" s="389"/>
-      <c r="AA18" s="389"/>
-      <c r="AB18" s="389"/>
-      <c r="AC18" s="389"/>
-      <c r="AD18" s="389"/>
-      <c r="AE18" s="389"/>
-      <c r="AF18" s="389"/>
-      <c r="AG18" s="389"/>
-      <c r="AH18" s="389"/>
-      <c r="AI18" s="389"/>
-      <c r="AJ18" s="389"/>
-      <c r="AK18" s="389"/>
-      <c r="AL18" s="389"/>
-      <c r="AM18" s="389"/>
-      <c r="AN18" s="389"/>
-      <c r="AO18" s="389"/>
-      <c r="AP18" s="389"/>
-      <c r="AQ18" s="389"/>
-      <c r="AR18" s="389"/>
-      <c r="AS18" s="389"/>
-      <c r="AT18" s="389"/>
-      <c r="AU18" s="389"/>
-      <c r="AV18" s="389"/>
-      <c r="AW18" s="389"/>
-      <c r="AX18" s="389"/>
-      <c r="AY18" s="389"/>
-      <c r="AZ18" s="389"/>
-      <c r="BA18" s="389"/>
-      <c r="BB18" s="389"/>
-      <c r="BC18" s="389"/>
-      <c r="BD18" s="389"/>
-      <c r="BE18" s="389"/>
-      <c r="BF18" s="389"/>
-      <c r="BG18" s="389"/>
-      <c r="BH18" s="389"/>
-      <c r="BI18" s="389"/>
-      <c r="BJ18" s="389"/>
-      <c r="BK18" s="389"/>
-      <c r="BL18" s="389"/>
-      <c r="BM18" s="389"/>
-      <c r="BN18" s="389"/>
-      <c r="BO18" s="389"/>
-      <c r="BP18" s="389"/>
-      <c r="BQ18" s="389"/>
-      <c r="BR18" s="389"/>
-      <c r="BS18" s="389"/>
-      <c r="BT18" s="389"/>
-      <c r="BU18" s="389"/>
-      <c r="BV18" s="389"/>
-      <c r="BW18" s="389"/>
-      <c r="BX18" s="389"/>
-      <c r="BY18" s="389"/>
-      <c r="BZ18" s="389"/>
-      <c r="CA18" s="389"/>
-      <c r="CB18" s="389"/>
-      <c r="CC18" s="389"/>
-      <c r="CD18" s="389"/>
-      <c r="CE18" s="389"/>
-      <c r="CF18" s="389"/>
-      <c r="CG18" s="389"/>
-      <c r="CH18" s="389"/>
-      <c r="CI18" s="389"/>
-      <c r="CJ18" s="389"/>
-      <c r="CK18" s="389"/>
-      <c r="CL18" s="389"/>
-      <c r="CM18" s="389"/>
-      <c r="CN18" s="389"/>
-      <c r="CO18" s="389"/>
-      <c r="CP18" s="389"/>
-      <c r="CQ18" s="389"/>
-      <c r="CR18" s="389"/>
-      <c r="CS18" s="389"/>
-      <c r="CT18" s="389"/>
-      <c r="CU18" s="389"/>
-      <c r="CV18" s="389"/>
-      <c r="CW18" s="389"/>
-      <c r="CX18" s="389"/>
-      <c r="CY18" s="389"/>
-      <c r="CZ18" s="389"/>
-      <c r="DA18" s="389"/>
-      <c r="DB18" s="389"/>
-      <c r="DC18" s="389"/>
-      <c r="DD18" s="389"/>
-      <c r="DE18" s="389"/>
-      <c r="DF18" s="389"/>
-      <c r="DG18" s="389"/>
-      <c r="DH18" s="389"/>
-      <c r="DI18" s="389"/>
-      <c r="DJ18" s="389"/>
-      <c r="DK18" s="389"/>
-      <c r="DL18" s="389"/>
-      <c r="DM18" s="389"/>
-      <c r="DN18" s="389"/>
-      <c r="DO18" s="389"/>
-      <c r="DP18" s="389"/>
-      <c r="DQ18" s="389"/>
-      <c r="DR18" s="389"/>
-      <c r="DS18" s="389"/>
-      <c r="DT18" s="389"/>
-      <c r="DU18" s="389"/>
-      <c r="DV18" s="389"/>
-      <c r="DW18" s="389"/>
-      <c r="DX18" s="389"/>
-      <c r="DY18" s="389"/>
-      <c r="DZ18" s="389"/>
-      <c r="EA18" s="389"/>
-      <c r="EB18" s="389"/>
-      <c r="EC18" s="389"/>
-      <c r="ED18" s="389"/>
-      <c r="EE18" s="389"/>
-      <c r="EF18" s="389"/>
-      <c r="EG18" s="389"/>
-      <c r="EH18" s="389"/>
-      <c r="EI18" s="389"/>
-      <c r="EJ18" s="389"/>
-      <c r="EK18" s="389"/>
     </row>
     <row r="19" spans="1:141" s="432" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="462">
@@ -37493,7 +37498,7 @@
         <v>983</v>
       </c>
       <c r="D19" s="385" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="E19" s="493" t="s">
         <v>776</v>
@@ -37511,12 +37516,12 @@
         <v>983</v>
       </c>
       <c r="D20" s="385" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="E20" s="493" t="s">
         <v>776</v>
       </c>
-      <c r="F20" s="494" t="s">
+      <c r="F20" s="430" t="s">
         <v>339</v>
       </c>
     </row>
@@ -37529,12 +37534,12 @@
         <v>983</v>
       </c>
       <c r="D21" s="385" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="E21" s="493" t="s">
         <v>776</v>
       </c>
-      <c r="F21" s="430" t="s">
+      <c r="F21" s="494" t="s">
         <v>339</v>
       </c>
     </row>
@@ -37547,12 +37552,12 @@
         <v>983</v>
       </c>
       <c r="D22" s="385" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E22" s="493" t="s">
         <v>776</v>
       </c>
-      <c r="F22" s="494" t="s">
+      <c r="F22" s="430" t="s">
         <v>339</v>
       </c>
     </row>
@@ -37565,12 +37570,12 @@
         <v>983</v>
       </c>
       <c r="D23" s="385" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="E23" s="493" t="s">
         <v>776</v>
       </c>
-      <c r="F23" s="430" t="s">
+      <c r="F23" s="494" t="s">
         <v>339</v>
       </c>
     </row>
@@ -37583,7 +37588,7 @@
         <v>983</v>
       </c>
       <c r="D24" s="385" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="E24" s="493" t="s">
         <v>776</v>
@@ -37592,21 +37597,21 @@
         <v>339</v>
       </c>
     </row>
-    <row r="25" spans="1:141" s="432" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="462">
-        <v>42736</v>
-      </c>
-      <c r="B25" s="465"/>
-      <c r="C25" s="464" t="s">
-        <v>983</v>
-      </c>
-      <c r="D25" s="385" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E25" s="493" t="s">
+    <row r="25" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="81"/>
+      <c r="C25" s="65" t="s">
+        <v>883</v>
+      </c>
+      <c r="D25" s="62" t="s">
+        <v>392</v>
+      </c>
+      <c r="E25" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F25" s="494" t="s">
+      <c r="F25" s="115" t="s">
         <v>339</v>
       </c>
     </row>
@@ -37616,7 +37621,7 @@
       </c>
       <c r="B26" s="81"/>
       <c r="C26" s="65" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="D26" s="62" t="s">
         <v>392</v>
@@ -37637,7 +37642,7 @@
         <v>884</v>
       </c>
       <c r="D27" s="62" t="s">
-        <v>392</v>
+        <v>546</v>
       </c>
       <c r="E27" s="134" t="s">
         <v>776</v>
@@ -37655,7 +37660,7 @@
         <v>884</v>
       </c>
       <c r="D28" s="62" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="E28" s="134" t="s">
         <v>776</v>
@@ -37673,7 +37678,7 @@
         <v>884</v>
       </c>
       <c r="D29" s="62" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E29" s="134" t="s">
         <v>776</v>
@@ -37691,7 +37696,7 @@
         <v>884</v>
       </c>
       <c r="D30" s="62" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E30" s="134" t="s">
         <v>776</v>
@@ -37700,16 +37705,16 @@
         <v>339</v>
       </c>
     </row>
-    <row r="31" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="60">
         <v>42736</v>
       </c>
       <c r="B31" s="81"/>
-      <c r="C31" s="65" t="s">
-        <v>884</v>
+      <c r="C31" s="62" t="s">
+        <v>885</v>
       </c>
       <c r="D31" s="62" t="s">
-        <v>552</v>
+        <v>392</v>
       </c>
       <c r="E31" s="134" t="s">
         <v>776</v>
@@ -37718,13 +37723,13 @@
         <v>339</v>
       </c>
     </row>
-    <row r="32" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="60">
         <v>42736</v>
       </c>
       <c r="B32" s="81"/>
       <c r="C32" s="62" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="D32" s="62" t="s">
         <v>392</v>
@@ -37737,20 +37742,20 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B33" s="81"/>
-      <c r="C33" s="62" t="s">
+      <c r="A33" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B33" s="84"/>
+      <c r="C33" s="68" t="s">
         <v>886</v>
       </c>
-      <c r="D33" s="62" t="s">
-        <v>392</v>
+      <c r="D33" s="68" t="s">
+        <v>555</v>
       </c>
       <c r="E33" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F33" s="115" t="s">
+      <c r="F33" s="119" t="s">
         <v>339</v>
       </c>
     </row>
@@ -37763,7 +37768,7 @@
         <v>886</v>
       </c>
       <c r="D34" s="68" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="E34" s="134" t="s">
         <v>776</v>
@@ -37781,7 +37786,7 @@
         <v>886</v>
       </c>
       <c r="D35" s="68" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E35" s="134" t="s">
         <v>776</v>
@@ -37790,7 +37795,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="66">
         <v>42736</v>
       </c>
@@ -37799,7 +37804,7 @@
         <v>886</v>
       </c>
       <c r="D36" s="68" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="E36" s="134" t="s">
         <v>776</v>
@@ -37809,39 +37814,39 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B37" s="84"/>
-      <c r="C37" s="68" t="s">
-        <v>886</v>
-      </c>
-      <c r="D37" s="68" t="s">
-        <v>561</v>
+      <c r="A37" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="81"/>
+      <c r="C37" s="62" t="s">
+        <v>888</v>
+      </c>
+      <c r="D37" s="62" t="s">
+        <v>392</v>
       </c>
       <c r="E37" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F37" s="119" t="s">
-        <v>339</v>
+      <c r="F37" s="115" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B38" s="81"/>
-      <c r="C38" s="62" t="s">
-        <v>888</v>
-      </c>
-      <c r="D38" s="62" t="s">
+      <c r="A38" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B38" s="84"/>
+      <c r="C38" s="84" t="s">
+        <v>887</v>
+      </c>
+      <c r="D38" s="65" t="s">
         <v>392</v>
       </c>
       <c r="E38" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F38" s="115" t="s">
-        <v>354</v>
+      <c r="F38" s="119" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -37852,8 +37857,8 @@
       <c r="C39" s="84" t="s">
         <v>887</v>
       </c>
-      <c r="D39" s="65" t="s">
-        <v>392</v>
+      <c r="D39" s="118" t="s">
+        <v>563</v>
       </c>
       <c r="E39" s="134" t="s">
         <v>776</v>
@@ -37871,7 +37876,7 @@
         <v>887</v>
       </c>
       <c r="D40" s="118" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="E40" s="134" t="s">
         <v>776</v>
@@ -37885,11 +37890,11 @@
         <v>42736</v>
       </c>
       <c r="B41" s="84"/>
-      <c r="C41" s="84" t="s">
-        <v>887</v>
-      </c>
-      <c r="D41" s="118" t="s">
-        <v>567</v>
+      <c r="C41" s="65" t="s">
+        <v>889</v>
+      </c>
+      <c r="D41" s="68" t="s">
+        <v>392</v>
       </c>
       <c r="E41" s="134" t="s">
         <v>776</v>
@@ -37903,14 +37908,14 @@
         <v>42736</v>
       </c>
       <c r="B42" s="84"/>
-      <c r="C42" s="65" t="s">
-        <v>889</v>
-      </c>
-      <c r="D42" s="68" t="s">
+      <c r="C42" s="68" t="s">
+        <v>892</v>
+      </c>
+      <c r="D42" s="82" t="s">
         <v>392</v>
       </c>
-      <c r="E42" s="134" t="s">
-        <v>776</v>
+      <c r="E42" s="84" t="s">
+        <v>777</v>
       </c>
       <c r="F42" s="119" t="s">
         <v>339</v>
@@ -37925,13 +37930,13 @@
         <v>892</v>
       </c>
       <c r="D43" s="82" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E43" s="84" t="s">
         <v>777</v>
       </c>
       <c r="F43" s="119" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -37943,13 +37948,13 @@
         <v>892</v>
       </c>
       <c r="D44" s="82" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E44" s="84" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F44" s="119" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -37961,16 +37966,16 @@
         <v>892</v>
       </c>
       <c r="D45" s="82" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E45" s="84" t="s">
         <v>778</v>
       </c>
       <c r="F45" s="119" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="66">
         <v>42736</v>
       </c>
@@ -37978,14 +37983,14 @@
       <c r="C46" s="68" t="s">
         <v>892</v>
       </c>
-      <c r="D46" s="82" t="s">
-        <v>393</v>
+      <c r="D46" s="68" t="s">
+        <v>394</v>
       </c>
       <c r="E46" s="84" t="s">
         <v>778</v>
       </c>
       <c r="F46" s="119" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -38000,7 +38005,7 @@
         <v>394</v>
       </c>
       <c r="E47" s="84" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F47" s="119" t="s">
         <v>340</v>
@@ -38012,16 +38017,16 @@
       </c>
       <c r="B48" s="84"/>
       <c r="C48" s="68" t="s">
-        <v>892</v>
+        <v>1059</v>
       </c>
       <c r="D48" s="68" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E48" s="84" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F48" s="119" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -38033,7 +38038,7 @@
         <v>1059</v>
       </c>
       <c r="D49" s="68" t="s">
-        <v>392</v>
+        <v>941</v>
       </c>
       <c r="E49" s="84" t="s">
         <v>776</v>
@@ -38047,20 +38052,20 @@
         <v>42736</v>
       </c>
       <c r="B50" s="84"/>
-      <c r="C50" s="68" t="s">
-        <v>1059</v>
+      <c r="C50" s="65" t="s">
+        <v>890</v>
       </c>
       <c r="D50" s="68" t="s">
-        <v>941</v>
-      </c>
-      <c r="E50" s="84" t="s">
+        <v>392</v>
+      </c>
+      <c r="E50" s="134" t="s">
         <v>776</v>
       </c>
       <c r="F50" s="119" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="66">
         <v>42736</v>
       </c>
@@ -38069,7 +38074,7 @@
         <v>890</v>
       </c>
       <c r="D51" s="68" t="s">
-        <v>392</v>
+        <v>729</v>
       </c>
       <c r="E51" s="134" t="s">
         <v>776</v>
@@ -38079,20 +38084,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B52" s="84"/>
-      <c r="C52" s="65" t="s">
+      <c r="A52" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B52" s="90"/>
+      <c r="C52" s="73" t="s">
         <v>890</v>
       </c>
-      <c r="D52" s="68" t="s">
-        <v>729</v>
-      </c>
-      <c r="E52" s="134" t="s">
+      <c r="D52" s="86" t="s">
+        <v>732</v>
+      </c>
+      <c r="E52" s="195" t="s">
         <v>776</v>
       </c>
-      <c r="F52" s="119" t="s">
+      <c r="F52" s="125" t="s">
         <v>339</v>
       </c>
     </row>
@@ -38100,12 +38105,12 @@
       <c r="A53" s="71">
         <v>42736</v>
       </c>
-      <c r="B53" s="90"/>
-      <c r="C53" s="73" t="s">
-        <v>890</v>
-      </c>
-      <c r="D53" s="86" t="s">
-        <v>732</v>
+      <c r="B53" s="69"/>
+      <c r="C53" s="65" t="s">
+        <v>891</v>
+      </c>
+      <c r="D53" s="82" t="s">
+        <v>834</v>
       </c>
       <c r="E53" s="195" t="s">
         <v>776</v>
@@ -38123,7 +38128,7 @@
         <v>891</v>
       </c>
       <c r="D54" s="82" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="E54" s="195" t="s">
         <v>776</v>
@@ -38141,7 +38146,7 @@
         <v>891</v>
       </c>
       <c r="D55" s="82" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="E55" s="195" t="s">
         <v>776</v>
@@ -38154,12 +38159,12 @@
       <c r="A56" s="71">
         <v>42736</v>
       </c>
-      <c r="B56" s="69"/>
+      <c r="B56" s="72"/>
       <c r="C56" s="65" t="s">
         <v>891</v>
       </c>
-      <c r="D56" s="82" t="s">
-        <v>839</v>
+      <c r="D56" s="88" t="s">
+        <v>841</v>
       </c>
       <c r="E56" s="195" t="s">
         <v>776</v>
@@ -38169,56 +38174,38 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="71">
-        <v>42736</v>
-      </c>
-      <c r="B57" s="72"/>
-      <c r="C57" s="65" t="s">
-        <v>891</v>
-      </c>
-      <c r="D57" s="88" t="s">
-        <v>841</v>
-      </c>
-      <c r="E57" s="195" t="s">
-        <v>776</v>
-      </c>
-      <c r="F57" s="125" t="s">
+      <c r="A57" s="263">
+        <v>42736</v>
+      </c>
+      <c r="B57" s="419"/>
+      <c r="C57" s="73" t="s">
+        <v>882</v>
+      </c>
+      <c r="D57" s="265" t="s">
+        <v>392</v>
+      </c>
+      <c r="E57" s="418" t="s">
+        <v>943</v>
+      </c>
+      <c r="F57" s="266" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="263">
-        <v>42736</v>
-      </c>
-      <c r="B58" s="419"/>
-      <c r="C58" s="73" t="s">
+      <c r="A58" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B58" s="81"/>
+      <c r="C58" s="62" t="s">
         <v>882</v>
       </c>
-      <c r="D58" s="265" t="s">
-        <v>392</v>
+      <c r="D58" s="65" t="s">
+        <v>941</v>
       </c>
       <c r="E58" s="418" t="s">
         <v>943</v>
       </c>
-      <c r="F58" s="266" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B59" s="81"/>
-      <c r="C59" s="62" t="s">
-        <v>882</v>
-      </c>
-      <c r="D59" s="65" t="s">
-        <v>941</v>
-      </c>
-      <c r="E59" s="418" t="s">
-        <v>943</v>
-      </c>
-      <c r="F59" s="115" t="s">
+      <c r="F58" s="115" t="s">
         <v>339</v>
       </c>
     </row>

</xml_diff>